<commit_message>
functional interaction and cytokine validation updates
</commit_message>
<xml_diff>
--- a/src/6_functional_interaction/results/clustering_nde75ntotal50_reg_and_downstream.xlsx
+++ b/src/6_functional_interaction/results/clustering_nde75ntotal50_reg_and_downstream.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rzhu/Gladstone Dropbox/Ronghui Zhu/GRNPerturbSeq/4_codes/GWT_perturbseq_analysis/src/6_functional_interaction/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905812FE-CC75-484F-857D-0C01410D9157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29835D6C-02B0-8B4E-9264-7F7AC7B8AFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{AE44F2CC-892D-F147-8D31-099354A290F9}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{AE44F2CC-892D-F147-8D31-099354A290F9}"/>
   </bookViews>
   <sheets>
     <sheet name="clustering_nde75ntotal50_reg_an" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2986" uniqueCount="2333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2987" uniqueCount="2331">
   <si>
     <t>cluster</t>
   </si>
@@ -6928,9 +6928,6 @@
     <t>upstream of cell cycle</t>
   </si>
   <si>
-    <t>upstream of mRNA processing</t>
-  </si>
-  <si>
     <t>ribosomal and mitochrondrial function</t>
   </si>
   <si>
@@ -6974,9 +6971,6 @@
   </si>
   <si>
     <t>Arp2/3 and CCC complex</t>
-  </si>
-  <si>
-    <t>upstream of interferon-stimulated genes</t>
   </si>
   <si>
     <t>MCTS1/DENR complex</t>
@@ -7863,13 +7857,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA81DAE6-2760-9145-ACBD-851BF9FC920B}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:CX113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AX1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
       <selection activeCell="A46" sqref="A46"/>
-      <selection pane="topRight" activeCell="AX48" sqref="AX48"/>
+      <selection pane="topRight" activeCell="AB29" sqref="AB29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8465,12 +8458,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2320</v>
+        <v>2318</v>
       </c>
       <c r="C3">
         <v>0.33187471312897199</v>
@@ -8961,12 +8954,12 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>2319</v>
+        <v>2317</v>
       </c>
       <c r="C5">
         <v>0.31559423959890698</v>
@@ -9221,7 +9214,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -9460,12 +9453,12 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>2318</v>
+        <v>2316</v>
       </c>
       <c r="C7">
         <v>0.42656591588091602</v>
@@ -9943,7 +9936,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>2310</v>
+        <v>2309</v>
       </c>
       <c r="C9">
         <v>0.33089423481331598</v>
@@ -10219,12 +10212,12 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>2307</v>
+        <v>2306</v>
       </c>
       <c r="C10">
         <v>0.22911499577717601</v>
@@ -10487,7 +10480,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="C11">
         <v>0.359497641102835</v>
@@ -10792,7 +10785,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="C12">
         <v>0.33679486415620702</v>
@@ -11092,12 +11085,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="13" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>2321</v>
+        <v>2319</v>
       </c>
       <c r="C13">
         <v>0.45555326108433197</v>
@@ -11394,10 +11387,13 @@
         <v>374</v>
       </c>
     </row>
-    <row r="14" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
+      <c r="B14" t="s">
+        <v>2297</v>
+      </c>
       <c r="C14">
         <v>0.25888600220628399</v>
       </c>
@@ -11564,7 +11560,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="15" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -12005,7 +12001,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>2302</v>
+        <v>2301</v>
       </c>
       <c r="C17">
         <v>0.36669567956120902</v>
@@ -12305,12 +12301,12 @@
         <v>452</v>
       </c>
     </row>
-    <row r="18" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>2322</v>
+        <v>2320</v>
       </c>
       <c r="C18">
         <v>0.293557487955523</v>
@@ -12565,7 +12561,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="19" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -12783,12 +12779,12 @@
         <v>494</v>
       </c>
     </row>
-    <row r="20" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>2323</v>
+        <v>2321</v>
       </c>
       <c r="C20">
         <v>0.36268442473992901</v>
@@ -12956,7 +12952,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="21" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -13237,12 +13233,12 @@
         <v>529</v>
       </c>
     </row>
-    <row r="22" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>2324</v>
+        <v>2322</v>
       </c>
       <c r="C22">
         <v>0.28963155622348602</v>
@@ -13502,7 +13498,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>2331</v>
+        <v>2329</v>
       </c>
       <c r="C23">
         <v>0.243696292158148</v>
@@ -13810,7 +13806,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>2331</v>
+        <v>2329</v>
       </c>
       <c r="C24">
         <v>0.81701690773941604</v>
@@ -14358,7 +14354,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="26" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -14621,7 +14617,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="27" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -14797,12 +14793,12 @@
         <v>671</v>
       </c>
     </row>
-    <row r="28" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>2300</v>
+        <v>2297</v>
       </c>
       <c r="C28">
         <v>0.15741562892331601</v>
@@ -15065,7 +15061,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>2301</v>
+        <v>2297</v>
       </c>
       <c r="C29">
         <v>0.38377081501144999</v>
@@ -15370,7 +15366,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>2302</v>
+        <v>2301</v>
       </c>
       <c r="C30">
         <v>0.28875117220896401</v>
@@ -15670,7 +15666,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="31" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -15864,7 +15860,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="32" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -16745,7 +16741,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>2308</v>
+        <v>2307</v>
       </c>
       <c r="C35">
         <v>0.28171518806627899</v>
@@ -17026,7 +17022,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>2307</v>
+        <v>2306</v>
       </c>
       <c r="C36">
         <v>0.29201454818350397</v>
@@ -17284,7 +17280,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="37" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -17552,7 +17548,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>2306</v>
+        <v>2305</v>
       </c>
       <c r="C38">
         <v>0.34560660919595299</v>
@@ -17828,12 +17824,12 @@
         <v>917</v>
       </c>
     </row>
-    <row r="39" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>2303</v>
+        <v>2302</v>
       </c>
       <c r="C39">
         <v>0.20867600505456699</v>
@@ -18130,12 +18126,12 @@
         <v>942</v>
       </c>
     </row>
-    <row r="40" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>2304</v>
+        <v>2303</v>
       </c>
       <c r="C40">
         <v>0.196843505767303</v>
@@ -18411,7 +18407,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="41" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -18671,7 +18667,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="42" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -18910,12 +18906,12 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="43" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>2305</v>
+        <v>2304</v>
       </c>
       <c r="C43">
         <v>0.20565669431647299</v>
@@ -19215,7 +19211,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="44" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -19454,12 +19450,12 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="45" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>2325</v>
+        <v>2323</v>
       </c>
       <c r="C45">
         <v>0.236207085886986</v>
@@ -19896,7 +19892,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="47" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
@@ -20621,7 +20617,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>2313</v>
+        <v>2312</v>
       </c>
       <c r="C50">
         <v>0.30356784142301102</v>
@@ -20924,7 +20920,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="51" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
@@ -21097,12 +21093,12 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="52" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>2311</v>
+        <v>2310</v>
       </c>
       <c r="C52">
         <v>0.14011492895462199</v>
@@ -21402,7 +21398,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="53" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
@@ -21889,7 +21885,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="55" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
@@ -22062,7 +22058,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="56" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
@@ -22367,12 +22363,12 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="57" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>2326</v>
+        <v>2324</v>
       </c>
       <c r="C57">
         <v>6.9709634939680395E-2</v>
@@ -22561,12 +22557,12 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="58" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>2327</v>
+        <v>2325</v>
       </c>
       <c r="C58">
         <v>0.329248779896197</v>
@@ -22800,7 +22796,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="59" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
@@ -23068,7 +23064,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>2302</v>
+        <v>2301</v>
       </c>
       <c r="C60">
         <v>0.37556242770235099</v>
@@ -23371,7 +23367,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="61" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
@@ -24354,7 +24350,7 @@
         <v>1446</v>
       </c>
     </row>
-    <row r="65" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
@@ -24575,7 +24571,7 @@
         <v>1462</v>
       </c>
     </row>
-    <row r="66" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
@@ -24801,7 +24797,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>2312</v>
+        <v>2311</v>
       </c>
       <c r="C67">
         <v>0.349621973181024</v>
@@ -25067,7 +25063,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>2312</v>
+        <v>2311</v>
       </c>
       <c r="C68">
         <v>0.38048197501055703</v>
@@ -25328,7 +25324,7 @@
         <v>1512</v>
       </c>
     </row>
-    <row r="69" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>67</v>
       </c>
@@ -25569,7 +25565,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>2313</v>
+        <v>2312</v>
       </c>
       <c r="C70">
         <v>0.30641795900885499</v>
@@ -25872,7 +25868,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="71" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
@@ -26093,12 +26089,12 @@
         <v>1571</v>
       </c>
     </row>
-    <row r="72" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>2328</v>
+        <v>2326</v>
       </c>
       <c r="C72">
         <v>0.17737589099291001</v>
@@ -26353,12 +26349,12 @@
         <v>1591</v>
       </c>
     </row>
-    <row r="73" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>2329</v>
+        <v>2327</v>
       </c>
       <c r="C73">
         <v>0.24507685653842901</v>
@@ -26574,7 +26570,7 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="74" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>72</v>
       </c>
@@ -26750,12 +26746,12 @@
         <v>1618</v>
       </c>
     </row>
-    <row r="75" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>2330</v>
+        <v>2328</v>
       </c>
       <c r="C75">
         <v>0.117556063528028</v>
@@ -27410,7 +27406,7 @@
         <v>1668</v>
       </c>
     </row>
-    <row r="78" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>76</v>
       </c>
@@ -28262,7 +28258,7 @@
         <v>1731</v>
       </c>
     </row>
-    <row r="81" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>79</v>
       </c>
@@ -28525,7 +28521,7 @@
         <v>1756</v>
       </c>
     </row>
-    <row r="82" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>80</v>
       </c>
@@ -28811,7 +28807,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>2332</v>
+        <v>2330</v>
       </c>
       <c r="C83">
         <v>0.31752870511929099</v>
@@ -29087,7 +29083,7 @@
         <v>1801</v>
       </c>
     </row>
-    <row r="84" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>82</v>
       </c>
@@ -29513,7 +29509,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>2300</v>
+        <v>2297</v>
       </c>
       <c r="C86">
         <v>0.33937074614888801</v>
@@ -29708,7 +29704,7 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="87" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>85</v>
       </c>
@@ -29947,7 +29943,7 @@
         <v>1862</v>
       </c>
     </row>
-    <row r="88" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>86</v>
       </c>
@@ -30207,12 +30203,12 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="89" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
       <c r="C89">
         <v>0.23813314818506301</v>
@@ -30515,12 +30511,12 @@
         <v>1912</v>
       </c>
     </row>
-    <row r="90" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>2300</v>
+        <v>2297</v>
       </c>
       <c r="C90">
         <v>0.178977419660517</v>
@@ -30820,7 +30816,7 @@
         <v>1936</v>
       </c>
     </row>
-    <row r="91" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>89</v>
       </c>
@@ -31062,7 +31058,7 @@
         <v>1951</v>
       </c>
     </row>
-    <row r="92" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>90</v>
       </c>
@@ -31572,7 +31568,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>2300</v>
+        <v>2297</v>
       </c>
       <c r="C94">
         <v>0.26018997117359399</v>
@@ -31743,12 +31739,12 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="95" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>2317</v>
+        <v>2297</v>
       </c>
       <c r="C95">
         <v>0.22179961284967301</v>
@@ -31967,7 +31963,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="96" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>94</v>
       </c>
@@ -32161,7 +32157,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="97" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>95</v>
       </c>
@@ -32445,7 +32441,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="98" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>96</v>
       </c>
@@ -32753,7 +32749,7 @@
         <v>2056</v>
       </c>
     </row>
-    <row r="99" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>97</v>
       </c>
@@ -33137,7 +33133,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>2331</v>
+        <v>2329</v>
       </c>
       <c r="C101">
         <v>0.27287871752600401</v>
@@ -33437,7 +33433,7 @@
         <v>2099</v>
       </c>
     </row>
-    <row r="102" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>100</v>
       </c>
@@ -34521,7 +34517,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>2300</v>
+        <v>2297</v>
       </c>
       <c r="C106">
         <v>0.36253454317748002</v>
@@ -34718,7 +34714,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>2300</v>
+        <v>2297</v>
       </c>
       <c r="C107">
         <v>0.34850601633467299</v>
@@ -34960,7 +34956,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>2300</v>
+        <v>2297</v>
       </c>
       <c r="C108">
         <v>0.277615743820811</v>
@@ -35462,7 +35458,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>2315</v>
+        <v>2314</v>
       </c>
       <c r="C110">
         <v>0.28925918259135902</v>
@@ -36007,7 +36003,7 @@
         <v>2266</v>
       </c>
     </row>
-    <row r="112" spans="1:102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>110</v>
       </c>
@@ -36188,7 +36184,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>2316</v>
+        <v>2315</v>
       </c>
       <c r="C113">
         <v>0.34201820539136801</v>
@@ -36492,43 +36488,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CX113" xr:uid="{DA81DAE6-2760-9145-ACBD-851BF9FC920B}">
-    <filterColumn colId="2">
-      <customFilters>
-        <customFilter operator="greaterThan" val="0.24"/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <filters>
-        <filter val="10"/>
-        <filter val="11"/>
-        <filter val="12"/>
-        <filter val="13"/>
-        <filter val="135"/>
-        <filter val="15"/>
-        <filter val="174"/>
-        <filter val="19"/>
-        <filter val="195"/>
-        <filter val="215"/>
-        <filter val="22"/>
-        <filter val="31"/>
-        <filter val="34"/>
-        <filter val="36"/>
-        <filter val="4"/>
-        <filter val="42"/>
-        <filter val="49"/>
-        <filter val="50"/>
-        <filter val="58"/>
-        <filter val="6"/>
-        <filter val="7"/>
-        <filter val="70"/>
-        <filter val="8"/>
-        <filter val="84"/>
-        <filter val="88"/>
-        <filter val="9"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:CX113" xr:uid="{DA81DAE6-2760-9145-ACBD-851BF9FC920B}"/>
   <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="colorScale" priority="2">
       <colorScale>

</xml_diff>

<commit_message>
updates to functional interaction analysis
</commit_message>
<xml_diff>
--- a/src/6_functional_interaction/results/clustering_nde75ntotal50_reg_and_downstream.xlsx
+++ b/src/6_functional_interaction/results/clustering_nde75ntotal50_reg_and_downstream.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rzhu/Gladstone Dropbox/Ronghui Zhu/GRNPerturbSeq/4_codes/GWT_perturbseq_analysis/src/6_functional_interaction/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29835D6C-02B0-8B4E-9264-7F7AC7B8AFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9189C017-9FF9-7646-B9BC-7AD70ED023AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{AE44F2CC-892D-F147-8D31-099354A290F9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{AE44F2CC-892D-F147-8D31-099354A290F9}"/>
   </bookViews>
   <sheets>
     <sheet name="clustering_nde75ntotal50_reg_an" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2987" uniqueCount="2331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2987" uniqueCount="2332">
   <si>
     <t>cluster</t>
   </si>
@@ -7016,6 +7016,9 @@
   </si>
   <si>
     <t>core BAF subunits</t>
+  </si>
+  <si>
+    <t>Th17 differentiation</t>
   </si>
 </sst>
 </file>
@@ -7860,9 +7863,9 @@
   <dimension ref="A1:CX113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A46" sqref="A46"/>
-      <selection pane="topRight" activeCell="AB29" sqref="AB29"/>
+      <selection pane="topRight" activeCell="A104" sqref="A104:XFD104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28263,7 +28266,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>2297</v>
+        <v>2331</v>
       </c>
       <c r="C81">
         <v>0.176930782308027</v>

</xml_diff>